<commit_message>
corrected invalid formula for total use
</commit_message>
<xml_diff>
--- a/NMxTotalUsexAccuracy/data/NMxPositiveAccuracy_anova.xlsx
+++ b/NMxTotalUsexAccuracy/data/NMxPositiveAccuracy_anova.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/neuromelanin/NMxAccuracy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/neuromelanin/NMxTotalUsexAccuracy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F90551-BE8B-DC44-9948-42DD9784C1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55433F8-9CCD-7246-BA17-B9930C14EE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28300" yWindow="1300" windowWidth="22080" windowHeight="14780" xr2:uid="{79B66A3E-72FC-BE4A-89D9-CD830D2D4145}"/>
   </bookViews>
@@ -354,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -366,12 +366,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -389,6 +383,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,65 +700,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31723B7A-45ED-944A-9BE0-99732653F64A}">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="P1" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="Q1" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="15" t="s">
         <v>48</v>
       </c>
     </row>
@@ -774,15 +769,14 @@
       <c r="B2" s="9">
         <v>7.0149834110000002</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="11">
         <v>6.6323999999999996</v>
       </c>
       <c r="D2" s="3">
         <v>20</v>
       </c>
-      <c r="E2" s="11">
-        <f>SUM(A2,B2,D2)</f>
-        <v>27.014983410999999</v>
+      <c r="E2" s="18">
+        <v>24</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -841,9 +835,8 @@
       <c r="D3" s="3">
         <v>23</v>
       </c>
-      <c r="E3" s="11">
-        <f t="shared" ref="E3:E66" si="3">SUM(A3,B3,D3)</f>
-        <v>28.283762746000001</v>
+      <c r="E3" s="18">
+        <v>57</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -877,7 +870,7 @@
         <v>-4.4757000000000005E-2</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P66" si="4">AVERAGE(M3,N3)</f>
+        <f t="shared" ref="P3:P66" si="3">AVERAGE(M3,N3)</f>
         <v>1.8258999999999997E-2</v>
       </c>
       <c r="Q3">
@@ -902,9 +895,8 @@
       <c r="D4" s="3">
         <v>26</v>
       </c>
-      <c r="E4" s="11">
-        <f t="shared" si="3"/>
-        <v>37.89285005</v>
+      <c r="E4" s="18">
+        <v>23</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -938,7 +930,7 @@
         <v>-8.9199000000000001E-2</v>
       </c>
       <c r="P4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-1.5273E-2</v>
       </c>
       <c r="Q4">
@@ -963,9 +955,8 @@
       <c r="D5" s="3">
         <v>34</v>
       </c>
-      <c r="E5" s="11">
-        <f t="shared" si="3"/>
-        <v>41.470071554999997</v>
+      <c r="E5" s="18">
+        <v>52</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -999,7 +990,7 @@
         <v>-2.5585499999999997E-2</v>
       </c>
       <c r="P5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.7536999999999995E-2</v>
       </c>
       <c r="Q5">
@@ -1024,9 +1015,8 @@
       <c r="D6" s="3">
         <v>21</v>
       </c>
-      <c r="E6" s="11">
-        <f t="shared" si="3"/>
-        <v>30.892294937999999</v>
+      <c r="E6" s="18">
+        <v>28</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -1060,7 +1050,7 @@
         <v>-0.30197600000000002</v>
       </c>
       <c r="P6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4.5526000000000004E-2</v>
       </c>
       <c r="Q6">
@@ -1085,9 +1075,8 @@
       <c r="D7" s="3">
         <v>23</v>
       </c>
-      <c r="E7" s="11">
-        <f t="shared" si="3"/>
-        <v>33.030146940000002</v>
+      <c r="E7" s="18">
+        <v>1</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
@@ -1121,7 +1110,7 @@
         <v>-0.17773949999999999</v>
       </c>
       <c r="P7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-9.7758000000000012E-2</v>
       </c>
       <c r="Q7">
@@ -1146,9 +1135,8 @@
       <c r="D8" s="3">
         <v>23</v>
       </c>
-      <c r="E8" s="11">
-        <f t="shared" si="3"/>
-        <v>29.342077498999998</v>
+      <c r="E8" s="18">
+        <v>0</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -1182,7 +1170,7 @@
         <v>-4.2699500000000001E-2</v>
       </c>
       <c r="P8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5.3605000000000007E-3</v>
       </c>
       <c r="Q8">
@@ -1207,9 +1195,8 @@
       <c r="D9" s="3">
         <v>20</v>
       </c>
-      <c r="E9" s="11">
-        <f t="shared" si="3"/>
-        <v>24.688248938000001</v>
+      <c r="E9" s="18">
+        <v>28</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
@@ -1243,7 +1230,7 @@
         <v>1.8943499999999999E-2</v>
       </c>
       <c r="P9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6.595100000000001E-2</v>
       </c>
       <c r="Q9">
@@ -1268,9 +1255,8 @@
       <c r="D10" s="3">
         <v>19</v>
       </c>
-      <c r="E10" s="11">
-        <f t="shared" si="3"/>
-        <v>29.418130130000002</v>
+      <c r="E10" s="18">
+        <v>2</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
@@ -1304,7 +1290,7 @@
         <v>-1.8413499999999999E-2</v>
       </c>
       <c r="P10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.7177500000000002E-2</v>
       </c>
       <c r="Q10">
@@ -1329,9 +1315,8 @@
       <c r="D11" s="3">
         <v>18</v>
       </c>
-      <c r="E11" s="11">
-        <f t="shared" si="3"/>
-        <v>26.201286164999999</v>
+      <c r="E11" s="18">
+        <v>3</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
@@ -1365,7 +1350,7 @@
         <v>-3.0740999999999997E-2</v>
       </c>
       <c r="P11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.23769400000000002</v>
       </c>
       <c r="Q11">
@@ -1390,9 +1375,8 @@
       <c r="D12" s="3">
         <v>21</v>
       </c>
-      <c r="E12" s="11">
-        <f t="shared" si="3"/>
-        <v>32.849809</v>
+      <c r="E12" s="18">
+        <v>1</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
@@ -1426,7 +1410,7 @@
         <v>-0.235064</v>
       </c>
       <c r="P12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.136906</v>
       </c>
       <c r="Q12">
@@ -1451,9 +1435,8 @@
       <c r="D13" s="3">
         <v>21</v>
       </c>
-      <c r="E13" s="11">
-        <f t="shared" si="3"/>
-        <v>29.547309888000001</v>
+      <c r="E13" s="18">
+        <v>12</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
@@ -1487,7 +1470,7 @@
         <v>-0.27285700000000002</v>
       </c>
       <c r="P13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.22975400000000001</v>
       </c>
       <c r="Q13">
@@ -1512,9 +1495,8 @@
       <c r="D14" s="3">
         <v>19</v>
       </c>
-      <c r="E14" s="11">
-        <f t="shared" si="3"/>
-        <v>27.887442010999997</v>
+      <c r="E14" s="18">
+        <v>8</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
@@ -1548,7 +1530,7 @@
         <v>-8.2378000000000007E-2</v>
       </c>
       <c r="P14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.2757500000000001E-2</v>
       </c>
       <c r="Q14">
@@ -1573,9 +1555,8 @@
       <c r="D15" s="3">
         <v>19</v>
       </c>
-      <c r="E15" s="11">
-        <f t="shared" si="3"/>
-        <v>27.222968737000002</v>
+      <c r="E15" s="18">
+        <v>8</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
@@ -1609,7 +1590,7 @@
         <v>9.95085E-2</v>
       </c>
       <c r="P15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6.3800499999999996E-2</v>
       </c>
       <c r="Q15">
@@ -1634,9 +1615,8 @@
       <c r="D16" s="3">
         <v>21</v>
       </c>
-      <c r="E16" s="11">
-        <f t="shared" si="3"/>
-        <v>30.397520628000002</v>
+      <c r="E16" s="18">
+        <v>0</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
@@ -1670,7 +1650,7 @@
         <v>-4.1527000000000001E-2</v>
       </c>
       <c r="P16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-7.9314999999999997E-2</v>
       </c>
       <c r="Q16">
@@ -1695,9 +1675,8 @@
       <c r="D17" s="3">
         <v>18</v>
       </c>
-      <c r="E17" s="11">
-        <f t="shared" si="3"/>
-        <v>26.267269286999998</v>
+      <c r="E17" s="18">
+        <v>0</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
@@ -1731,7 +1710,7 @@
         <v>-0.1514675</v>
       </c>
       <c r="P17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-3.9558999999999997E-2</v>
       </c>
       <c r="Q17">
@@ -1756,9 +1735,8 @@
       <c r="D18" s="3">
         <v>20</v>
       </c>
-      <c r="E18" s="11">
-        <f t="shared" si="3"/>
-        <v>27.722397643000001</v>
+      <c r="E18" s="18">
+        <v>24</v>
       </c>
       <c r="F18" s="2">
         <v>0</v>
@@ -1792,7 +1770,7 @@
         <v>6.8585000000000007E-2</v>
       </c>
       <c r="P18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.7403E-2</v>
       </c>
       <c r="Q18">
@@ -1817,9 +1795,8 @@
       <c r="D19" s="3">
         <v>21</v>
       </c>
-      <c r="E19" s="11">
-        <f t="shared" si="3"/>
-        <v>33.399481039999998</v>
+      <c r="E19" s="18">
+        <v>0</v>
       </c>
       <c r="F19" s="2">
         <v>0</v>
@@ -1853,7 +1830,7 @@
         <v>-5.9248000000000002E-2</v>
       </c>
       <c r="P19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4.4795999999999996E-2</v>
       </c>
       <c r="Q19">
@@ -1878,9 +1855,8 @@
       <c r="D20" s="3">
         <v>20</v>
       </c>
-      <c r="E20" s="11">
-        <f t="shared" si="3"/>
-        <v>28.407680970999998</v>
+      <c r="E20" s="18">
+        <v>50</v>
       </c>
       <c r="F20" s="2">
         <v>0</v>
@@ -1914,7 +1890,7 @@
         <v>1.0822E-2</v>
       </c>
       <c r="P20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-1.7061E-2</v>
       </c>
       <c r="Q20">
@@ -1939,9 +1915,8 @@
       <c r="D21" s="3">
         <v>19</v>
       </c>
-      <c r="E21" s="11">
-        <f t="shared" si="3"/>
-        <v>27.538233206000001</v>
+      <c r="E21" s="18">
+        <v>32</v>
       </c>
       <c r="F21" s="2">
         <v>0</v>
@@ -1975,7 +1950,7 @@
         <v>0.1214655</v>
       </c>
       <c r="P21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4.6637499999999998E-2</v>
       </c>
       <c r="Q21">
@@ -2000,9 +1975,8 @@
       <c r="D22" s="3">
         <v>19</v>
       </c>
-      <c r="E22" s="11">
-        <f t="shared" si="3"/>
-        <v>28.547210065000002</v>
+      <c r="E22" s="18">
+        <v>0</v>
       </c>
       <c r="F22" s="2">
         <v>0</v>
@@ -2036,7 +2010,7 @@
         <v>-0.163326</v>
       </c>
       <c r="P22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.132187</v>
       </c>
       <c r="Q22">
@@ -2061,9 +2035,8 @@
       <c r="D23" s="3">
         <v>20</v>
       </c>
-      <c r="E23" s="11">
-        <f t="shared" si="3"/>
-        <v>25.649759837000001</v>
+      <c r="E23" s="18">
+        <v>32</v>
       </c>
       <c r="F23" s="2">
         <v>0</v>
@@ -2097,7 +2070,7 @@
         <v>-7.0611499999999994E-2</v>
       </c>
       <c r="P23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6.1749999999999999E-3</v>
       </c>
       <c r="Q23">
@@ -2122,9 +2095,8 @@
       <c r="D24" s="3">
         <v>19</v>
       </c>
-      <c r="E24" s="11">
-        <f t="shared" si="3"/>
-        <v>28.222083269999999</v>
+      <c r="E24" s="18">
+        <v>42</v>
       </c>
       <c r="F24" s="2">
         <v>0</v>
@@ -2158,7 +2130,7 @@
         <v>-9.2540499999999998E-2</v>
       </c>
       <c r="P24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.1017605</v>
       </c>
       <c r="Q24">
@@ -2183,9 +2155,8 @@
       <c r="D25" s="3">
         <v>22</v>
       </c>
-      <c r="E25" s="11">
-        <f t="shared" si="3"/>
-        <v>31.075425877000001</v>
+      <c r="E25" s="18">
+        <v>4</v>
       </c>
       <c r="F25" s="2">
         <v>0</v>
@@ -2219,7 +2190,7 @@
         <v>-0.17187150000000001</v>
       </c>
       <c r="P25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.1010665</v>
       </c>
       <c r="Q25">
@@ -2244,9 +2215,8 @@
       <c r="D26" s="3">
         <v>18</v>
       </c>
-      <c r="E26" s="11">
-        <f t="shared" si="3"/>
-        <v>30.455561510000003</v>
+      <c r="E26" s="18">
+        <v>25</v>
       </c>
       <c r="F26" s="2">
         <v>0</v>
@@ -2280,7 +2250,7 @@
         <v>-1.6561000000000003E-2</v>
       </c>
       <c r="P26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5.1922000000000003E-2</v>
       </c>
       <c r="Q26">
@@ -2305,9 +2275,8 @@
       <c r="D27" s="3">
         <v>32</v>
       </c>
-      <c r="E27" s="11">
-        <f t="shared" si="3"/>
-        <v>41.590708190000001</v>
+      <c r="E27" s="18">
+        <v>0</v>
       </c>
       <c r="F27" s="2">
         <v>0</v>
@@ -2341,7 +2310,7 @@
         <v>-0.162936</v>
       </c>
       <c r="P27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.14506449999999999</v>
       </c>
       <c r="Q27">
@@ -2366,9 +2335,8 @@
       <c r="D28" s="3">
         <v>20</v>
       </c>
-      <c r="E28" s="11">
-        <f t="shared" si="3"/>
-        <v>28.071761545000001</v>
+      <c r="E28" s="18">
+        <v>19</v>
       </c>
       <c r="F28" s="2">
         <v>0</v>
@@ -2402,7 +2370,7 @@
         <v>-0.15967600000000001</v>
       </c>
       <c r="P28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4.6128500000000003E-2</v>
       </c>
       <c r="Q28">
@@ -2427,9 +2395,8 @@
       <c r="D29" s="3">
         <v>20</v>
       </c>
-      <c r="E29" s="11">
-        <f t="shared" si="3"/>
-        <v>27.342681935999998</v>
+      <c r="E29" s="18">
+        <v>55</v>
       </c>
       <c r="F29" s="2">
         <v>0</v>
@@ -2463,7 +2430,7 @@
         <v>-4.1850999999999999E-2</v>
       </c>
       <c r="P29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.12528</v>
       </c>
       <c r="Q29">
@@ -2488,9 +2455,8 @@
       <c r="D30" s="3">
         <v>18</v>
       </c>
-      <c r="E30" s="11">
-        <f t="shared" si="3"/>
-        <v>24.414532676</v>
+      <c r="E30" s="18">
+        <v>3</v>
       </c>
       <c r="F30" s="2">
         <v>0</v>
@@ -2524,7 +2490,7 @@
         <v>-0.19819799999999999</v>
       </c>
       <c r="P30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-7.5264500000000012E-2</v>
       </c>
       <c r="Q30">
@@ -2549,9 +2515,8 @@
       <c r="D31" s="3">
         <v>35</v>
       </c>
-      <c r="E31" s="11">
-        <f t="shared" si="3"/>
-        <v>42.593527115999997</v>
+      <c r="E31" s="18">
+        <v>0</v>
       </c>
       <c r="F31" s="2">
         <v>0</v>
@@ -2585,7 +2550,7 @@
         <v>-0.19357799999999997</v>
       </c>
       <c r="P31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-1.7041999999999998E-2</v>
       </c>
       <c r="Q31">
@@ -2610,9 +2575,8 @@
       <c r="D32" s="3">
         <v>27</v>
       </c>
-      <c r="E32" s="11">
-        <f t="shared" si="3"/>
-        <v>33.086239947000003</v>
+      <c r="E32" s="18">
+        <v>43</v>
       </c>
       <c r="F32" s="2">
         <v>0</v>
@@ -2646,7 +2610,7 @@
         <v>2.3279000000000001E-2</v>
       </c>
       <c r="P32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-2.7189500000000002E-2</v>
       </c>
       <c r="Q32">
@@ -2671,9 +2635,8 @@
       <c r="D33" s="3">
         <v>21</v>
       </c>
-      <c r="E33" s="11">
-        <f t="shared" si="3"/>
-        <v>28.081494340999999</v>
+      <c r="E33" s="18">
+        <v>42</v>
       </c>
       <c r="F33" s="2">
         <v>0</v>
@@ -2707,7 +2670,7 @@
         <v>-0.140926</v>
       </c>
       <c r="P33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.13221749999999999</v>
       </c>
       <c r="Q33">
@@ -2732,9 +2695,8 @@
       <c r="D34" s="3">
         <v>22</v>
       </c>
-      <c r="E34" s="11">
-        <f t="shared" si="3"/>
-        <v>32.586067829999998</v>
+      <c r="E34" s="18">
+        <v>35</v>
       </c>
       <c r="F34" s="2">
         <v>0</v>
@@ -2764,19 +2726,19 @@
         <v>0.12664800000000001</v>
       </c>
       <c r="O34">
-        <f t="shared" ref="O34:O65" si="5">AVERAGE(G34,H34)</f>
+        <f t="shared" ref="O34:O65" si="4">AVERAGE(G34,H34)</f>
         <v>9.9430000000000004E-3</v>
       </c>
       <c r="P34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.12137000000000001</v>
       </c>
       <c r="Q34">
-        <f t="shared" ref="Q34:Q66" si="6">AVERAGE(K34,L34)</f>
+        <f t="shared" ref="Q34:Q66" si="5">AVERAGE(K34,L34)</f>
         <v>-0.21374500000000002</v>
       </c>
       <c r="R34">
-        <f t="shared" ref="R34:R66" si="7">AVERAGE(I34,J34)</f>
+        <f t="shared" ref="R34:R66" si="6">AVERAGE(I34,J34)</f>
         <v>-0.11158849999999999</v>
       </c>
     </row>
@@ -2793,9 +2755,8 @@
       <c r="D35" s="3">
         <v>23</v>
       </c>
-      <c r="E35" s="11">
-        <f t="shared" si="3"/>
-        <v>34.051443660000004</v>
+      <c r="E35" s="18">
+        <v>9</v>
       </c>
       <c r="F35" s="2">
         <v>0</v>
@@ -2825,19 +2786,19 @@
         <v>-8.1860000000000002E-2</v>
       </c>
       <c r="O35">
+        <f t="shared" si="4"/>
+        <v>-0.16462749999999998</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="3"/>
+        <v>-0.139573</v>
+      </c>
+      <c r="Q35">
         <f t="shared" si="5"/>
-        <v>-0.16462749999999998</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="4"/>
-        <v>-0.139573</v>
-      </c>
-      <c r="Q35">
+        <v>2.1119999999999993E-3</v>
+      </c>
+      <c r="R35">
         <f t="shared" si="6"/>
-        <v>2.1119999999999993E-3</v>
-      </c>
-      <c r="R35">
-        <f t="shared" si="7"/>
         <v>4.7274000000000004E-2</v>
       </c>
     </row>
@@ -2854,9 +2815,8 @@
       <c r="D36" s="10">
         <v>19</v>
       </c>
-      <c r="E36" s="11">
-        <f t="shared" si="3"/>
-        <v>25.456789682</v>
+      <c r="E36" s="18">
+        <v>26</v>
       </c>
       <c r="F36" s="2">
         <v>0</v>
@@ -2886,19 +2846,19 @@
         <v>6.8223000000000006E-2</v>
       </c>
       <c r="O36">
+        <f t="shared" si="4"/>
+        <v>5.8689999999999999E-2</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="3"/>
+        <v>6.0819499999999999E-2</v>
+      </c>
+      <c r="Q36">
         <f t="shared" si="5"/>
-        <v>5.8689999999999999E-2</v>
-      </c>
-      <c r="P36">
-        <f t="shared" si="4"/>
-        <v>6.0819499999999999E-2</v>
-      </c>
-      <c r="Q36">
+        <v>-4.3700000000000003E-2</v>
+      </c>
+      <c r="R36">
         <f t="shared" si="6"/>
-        <v>-4.3700000000000003E-2</v>
-      </c>
-      <c r="R36">
-        <f t="shared" si="7"/>
         <v>1.7628499999999998E-2</v>
       </c>
     </row>
@@ -2915,9 +2875,8 @@
       <c r="D37" s="3">
         <v>20</v>
       </c>
-      <c r="E37" s="11">
-        <f>SUM(A37,B37,D37)</f>
-        <v>27.014983410999999</v>
+      <c r="E37" s="18">
+        <v>24</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
@@ -2947,19 +2906,19 @@
         <v>6.9194000000000006E-2</v>
       </c>
       <c r="O37">
+        <f t="shared" si="4"/>
+        <v>-0.1300385</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="3"/>
+        <v>4.3566000000000001E-2</v>
+      </c>
+      <c r="Q37">
         <f t="shared" si="5"/>
-        <v>-0.1300385</v>
-      </c>
-      <c r="P37">
-        <f t="shared" si="4"/>
-        <v>4.3566000000000001E-2</v>
-      </c>
-      <c r="Q37">
+        <v>-2.8499E-2</v>
+      </c>
+      <c r="R37">
         <f t="shared" si="6"/>
-        <v>-2.8499E-2</v>
-      </c>
-      <c r="R37">
-        <f t="shared" si="7"/>
         <v>9.0135999999999994E-2</v>
       </c>
     </row>
@@ -2976,9 +2935,8 @@
       <c r="D38" s="3">
         <v>23</v>
       </c>
-      <c r="E38" s="11">
-        <f t="shared" si="3"/>
-        <v>28.283762746000001</v>
+      <c r="E38" s="18">
+        <v>57</v>
       </c>
       <c r="F38" s="2">
         <v>1</v>
@@ -3008,19 +2966,19 @@
         <v>9.2760999999999996E-2</v>
       </c>
       <c r="O38">
+        <f t="shared" si="4"/>
+        <v>0.20445249999999998</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="3"/>
+        <v>0.14322399999999999</v>
+      </c>
+      <c r="Q38">
         <f t="shared" si="5"/>
-        <v>0.20445249999999998</v>
-      </c>
-      <c r="P38">
-        <f t="shared" si="4"/>
-        <v>0.14322399999999999</v>
-      </c>
-      <c r="Q38">
+        <v>0.10961900000000001</v>
+      </c>
+      <c r="R38">
         <f t="shared" si="6"/>
-        <v>0.10961900000000001</v>
-      </c>
-      <c r="R38">
-        <f t="shared" si="7"/>
         <v>7.9495999999999997E-2</v>
       </c>
     </row>
@@ -3037,9 +2995,8 @@
       <c r="D39" s="3">
         <v>26</v>
       </c>
-      <c r="E39" s="11">
-        <f t="shared" si="3"/>
-        <v>37.89285005</v>
+      <c r="E39" s="18">
+        <v>23</v>
       </c>
       <c r="F39" s="2">
         <v>1</v>
@@ -3069,19 +3026,19 @@
         <v>-6.4127000000000003E-2</v>
       </c>
       <c r="O39">
+        <f t="shared" si="4"/>
+        <v>-0.1692205</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="3"/>
+        <v>-4.1827500000000004E-2</v>
+      </c>
+      <c r="Q39">
         <f t="shared" si="5"/>
-        <v>-0.1692205</v>
-      </c>
-      <c r="P39">
-        <f t="shared" si="4"/>
-        <v>-4.1827500000000004E-2</v>
-      </c>
-      <c r="Q39">
+        <v>0.13337350000000001</v>
+      </c>
+      <c r="R39">
         <f t="shared" si="6"/>
-        <v>0.13337350000000001</v>
-      </c>
-      <c r="R39">
-        <f t="shared" si="7"/>
         <v>0.12923599999999999</v>
       </c>
     </row>
@@ -3098,9 +3055,8 @@
       <c r="D40" s="3">
         <v>34</v>
       </c>
-      <c r="E40" s="11">
-        <f t="shared" si="3"/>
-        <v>41.470071554999997</v>
+      <c r="E40" s="18">
+        <v>52</v>
       </c>
       <c r="F40" s="2">
         <v>1</v>
@@ -3130,19 +3086,19 @@
         <v>9.3731999999999996E-2</v>
       </c>
       <c r="O40">
+        <f t="shared" si="4"/>
+        <v>0.2122675</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="3"/>
+        <v>8.5449499999999998E-2</v>
+      </c>
+      <c r="Q40">
         <f t="shared" si="5"/>
-        <v>0.2122675</v>
-      </c>
-      <c r="P40">
-        <f t="shared" si="4"/>
-        <v>8.5449499999999998E-2</v>
-      </c>
-      <c r="Q40">
+        <v>0.1814935</v>
+      </c>
+      <c r="R40">
         <f t="shared" si="6"/>
-        <v>0.1814935</v>
-      </c>
-      <c r="R40">
-        <f t="shared" si="7"/>
         <v>8.39255E-2</v>
       </c>
     </row>
@@ -3159,9 +3115,8 @@
       <c r="D41" s="3">
         <v>21</v>
       </c>
-      <c r="E41" s="11">
-        <f t="shared" si="3"/>
-        <v>30.892294937999999</v>
+      <c r="E41" s="18">
+        <v>28</v>
       </c>
       <c r="F41" s="2">
         <v>1</v>
@@ -3191,19 +3146,19 @@
         <v>-1.4874999999999999E-2</v>
       </c>
       <c r="O41">
+        <f t="shared" si="4"/>
+        <v>-0.14957500000000001</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="3"/>
+        <v>2.2869500000000001E-2</v>
+      </c>
+      <c r="Q41">
         <f t="shared" si="5"/>
-        <v>-0.14957500000000001</v>
-      </c>
-      <c r="P41">
-        <f t="shared" si="4"/>
-        <v>2.2869500000000001E-2</v>
-      </c>
-      <c r="Q41">
+        <v>0.15199850000000001</v>
+      </c>
+      <c r="R41">
         <f t="shared" si="6"/>
-        <v>0.15199850000000001</v>
-      </c>
-      <c r="R41">
-        <f t="shared" si="7"/>
         <v>0.19106049999999999</v>
       </c>
     </row>
@@ -3220,9 +3175,8 @@
       <c r="D42" s="3">
         <v>23</v>
       </c>
-      <c r="E42" s="11">
-        <f t="shared" si="3"/>
-        <v>33.030146940000002</v>
+      <c r="E42" s="18">
+        <v>1</v>
       </c>
       <c r="F42" s="2">
         <v>1</v>
@@ -3252,19 +3206,19 @@
         <v>7.8172000000000005E-2</v>
       </c>
       <c r="O42">
+        <f t="shared" si="4"/>
+        <v>2.5348500000000003E-2</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="3"/>
+        <v>3.6233500000000002E-2</v>
+      </c>
+      <c r="Q42">
         <f t="shared" si="5"/>
-        <v>2.5348500000000003E-2</v>
-      </c>
-      <c r="P42">
-        <f t="shared" si="4"/>
-        <v>3.6233500000000002E-2</v>
-      </c>
-      <c r="Q42">
+        <v>-4.3002499999999999E-2</v>
+      </c>
+      <c r="R42">
         <f t="shared" si="6"/>
-        <v>-4.3002499999999999E-2</v>
-      </c>
-      <c r="R42">
-        <f t="shared" si="7"/>
         <v>-1.8894000000000001E-2</v>
       </c>
     </row>
@@ -3281,9 +3235,8 @@
       <c r="D43" s="3">
         <v>23</v>
       </c>
-      <c r="E43" s="11">
-        <f t="shared" si="3"/>
-        <v>29.342077498999998</v>
+      <c r="E43" s="18">
+        <v>0</v>
       </c>
       <c r="F43" s="2">
         <v>1</v>
@@ -3313,19 +3266,19 @@
         <v>0.10079100000000001</v>
       </c>
       <c r="O43">
+        <f t="shared" si="4"/>
+        <v>2.6543500000000001E-2</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="3"/>
+        <v>5.2115500000000002E-2</v>
+      </c>
+      <c r="Q43">
         <f t="shared" si="5"/>
-        <v>2.6543500000000001E-2</v>
-      </c>
-      <c r="P43">
-        <f t="shared" si="4"/>
-        <v>5.2115500000000002E-2</v>
-      </c>
-      <c r="Q43">
+        <v>0.1353705</v>
+      </c>
+      <c r="R43">
         <f t="shared" si="6"/>
-        <v>0.1353705</v>
-      </c>
-      <c r="R43">
-        <f t="shared" si="7"/>
         <v>0.1074295</v>
       </c>
     </row>
@@ -3342,9 +3295,8 @@
       <c r="D44" s="3">
         <v>20</v>
       </c>
-      <c r="E44" s="11">
-        <f t="shared" si="3"/>
-        <v>24.688248938000001</v>
+      <c r="E44" s="18">
+        <v>28</v>
       </c>
       <c r="F44" s="2">
         <v>1</v>
@@ -3374,19 +3326,19 @@
         <v>7.3447999999999999E-2</v>
       </c>
       <c r="O44">
+        <f t="shared" si="4"/>
+        <v>3.6229499999999998E-2</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="3"/>
+        <v>5.1860999999999997E-2</v>
+      </c>
+      <c r="Q44">
         <f t="shared" si="5"/>
-        <v>3.6229499999999998E-2</v>
-      </c>
-      <c r="P44">
-        <f t="shared" si="4"/>
-        <v>5.1860999999999997E-2</v>
-      </c>
-      <c r="Q44">
+        <v>5.4734000000000005E-2</v>
+      </c>
+      <c r="R44">
         <f t="shared" si="6"/>
-        <v>5.4734000000000005E-2</v>
-      </c>
-      <c r="R44">
-        <f t="shared" si="7"/>
         <v>4.6152499999999999E-2</v>
       </c>
     </row>
@@ -3403,9 +3355,8 @@
       <c r="D45" s="3">
         <v>19</v>
       </c>
-      <c r="E45" s="11">
-        <f t="shared" si="3"/>
-        <v>29.418130130000002</v>
+      <c r="E45" s="18">
+        <v>2</v>
       </c>
       <c r="F45" s="2">
         <v>1</v>
@@ -3435,19 +3386,19 @@
         <v>3.0689999999999999E-2</v>
       </c>
       <c r="O45">
+        <f t="shared" si="4"/>
+        <v>-7.6849499999999987E-2</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="3"/>
+        <v>2.0375499999999998E-2</v>
+      </c>
+      <c r="Q45">
         <f t="shared" si="5"/>
-        <v>-7.6849499999999987E-2</v>
-      </c>
-      <c r="P45">
-        <f t="shared" si="4"/>
-        <v>2.0375499999999998E-2</v>
-      </c>
-      <c r="Q45">
+        <v>-7.6815500000000009E-2</v>
+      </c>
+      <c r="R45">
         <f t="shared" si="6"/>
-        <v>-7.6815500000000009E-2</v>
-      </c>
-      <c r="R45">
-        <f t="shared" si="7"/>
         <v>-7.0218000000000003E-2</v>
       </c>
     </row>
@@ -3464,9 +3415,8 @@
       <c r="D46" s="3">
         <v>18</v>
       </c>
-      <c r="E46" s="11">
-        <f t="shared" si="3"/>
-        <v>26.201286164999999</v>
+      <c r="E46" s="18">
+        <v>3</v>
       </c>
       <c r="F46" s="2">
         <v>1</v>
@@ -3496,19 +3446,19 @@
         <v>-2.0787E-2</v>
       </c>
       <c r="O46">
+        <f t="shared" si="4"/>
+        <v>0.13872950000000001</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="3"/>
+        <v>-3.7075999999999998E-2</v>
+      </c>
+      <c r="Q46">
         <f t="shared" si="5"/>
-        <v>0.13872950000000001</v>
-      </c>
-      <c r="P46">
-        <f t="shared" si="4"/>
-        <v>-3.7075999999999998E-2</v>
-      </c>
-      <c r="Q46">
+        <v>3.7094500000000002E-2</v>
+      </c>
+      <c r="R46">
         <f t="shared" si="6"/>
-        <v>3.7094500000000002E-2</v>
-      </c>
-      <c r="R46">
-        <f t="shared" si="7"/>
         <v>0.105819</v>
       </c>
     </row>
@@ -3525,9 +3475,8 @@
       <c r="D47" s="3">
         <v>21</v>
       </c>
-      <c r="E47" s="11">
-        <f t="shared" si="3"/>
-        <v>32.849809</v>
+      <c r="E47" s="18">
+        <v>1</v>
       </c>
       <c r="F47" s="2">
         <v>1</v>
@@ -3557,19 +3506,19 @@
         <v>-2.4535000000000001E-2</v>
       </c>
       <c r="O47">
+        <f t="shared" si="4"/>
+        <v>-9.6784000000000009E-2</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="3"/>
+        <v>-5.0932499999999999E-2</v>
+      </c>
+      <c r="Q47">
         <f t="shared" si="5"/>
-        <v>-9.6784000000000009E-2</v>
-      </c>
-      <c r="P47">
-        <f t="shared" si="4"/>
-        <v>-5.0932499999999999E-2</v>
-      </c>
-      <c r="Q47">
+        <v>8.2685499999999995E-2</v>
+      </c>
+      <c r="R47">
         <f t="shared" si="6"/>
-        <v>8.2685499999999995E-2</v>
-      </c>
-      <c r="R47">
-        <f t="shared" si="7"/>
         <v>0.17643049999999999</v>
       </c>
     </row>
@@ -3586,9 +3535,8 @@
       <c r="D48" s="3">
         <v>21</v>
       </c>
-      <c r="E48" s="11">
-        <f t="shared" si="3"/>
-        <v>29.547309888000001</v>
+      <c r="E48" s="18">
+        <v>12</v>
       </c>
       <c r="F48" s="2">
         <v>1</v>
@@ -3618,19 +3566,19 @@
         <v>0.11176899999999999</v>
       </c>
       <c r="O48">
+        <f t="shared" si="4"/>
+        <v>0.16839500000000002</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="3"/>
+        <v>0.10262099999999999</v>
+      </c>
+      <c r="Q48">
         <f t="shared" si="5"/>
-        <v>0.16839500000000002</v>
-      </c>
-      <c r="P48">
-        <f t="shared" si="4"/>
-        <v>0.10262099999999999</v>
-      </c>
-      <c r="Q48">
+        <v>9.5372499999999999E-2</v>
+      </c>
+      <c r="R48">
         <f t="shared" si="6"/>
-        <v>9.5372499999999999E-2</v>
-      </c>
-      <c r="R48">
-        <f t="shared" si="7"/>
         <v>-5.3498499999999997E-2</v>
       </c>
     </row>
@@ -3647,9 +3595,8 @@
       <c r="D49" s="3">
         <v>19</v>
       </c>
-      <c r="E49" s="11">
-        <f t="shared" si="3"/>
-        <v>27.887442010999997</v>
+      <c r="E49" s="18">
+        <v>8</v>
       </c>
       <c r="F49" s="2">
         <v>1</v>
@@ -3679,19 +3626,19 @@
         <v>5.8465000000000003E-2</v>
       </c>
       <c r="O49">
+        <f t="shared" si="4"/>
+        <v>0.1037415</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="3"/>
+        <v>3.4941E-2</v>
+      </c>
+      <c r="Q49">
         <f t="shared" si="5"/>
-        <v>0.1037415</v>
-      </c>
-      <c r="P49">
-        <f t="shared" si="4"/>
-        <v>3.4941E-2</v>
-      </c>
-      <c r="Q49">
+        <v>0.14825250000000001</v>
+      </c>
+      <c r="R49">
         <f t="shared" si="6"/>
-        <v>0.14825250000000001</v>
-      </c>
-      <c r="R49">
-        <f t="shared" si="7"/>
         <v>6.0884000000000008E-2</v>
       </c>
     </row>
@@ -3708,9 +3655,8 @@
       <c r="D50" s="3">
         <v>19</v>
       </c>
-      <c r="E50" s="11">
-        <f t="shared" si="3"/>
-        <v>27.222968737000002</v>
+      <c r="E50" s="18">
+        <v>8</v>
       </c>
       <c r="F50" s="2">
         <v>1</v>
@@ -3740,19 +3686,19 @@
         <v>0.23819199999999999</v>
       </c>
       <c r="O50">
+        <f t="shared" si="4"/>
+        <v>8.7649000000000005E-2</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="3"/>
+        <v>0.23391849999999997</v>
+      </c>
+      <c r="Q50">
         <f t="shared" si="5"/>
-        <v>8.7649000000000005E-2</v>
-      </c>
-      <c r="P50">
-        <f t="shared" si="4"/>
-        <v>0.23391849999999997</v>
-      </c>
-      <c r="Q50">
+        <v>-1.0112000000000001E-2</v>
+      </c>
+      <c r="R50">
         <f t="shared" si="6"/>
-        <v>-1.0112000000000001E-2</v>
-      </c>
-      <c r="R50">
-        <f t="shared" si="7"/>
         <v>9.77885E-2</v>
       </c>
     </row>
@@ -3769,9 +3715,8 @@
       <c r="D51" s="3">
         <v>21</v>
       </c>
-      <c r="E51" s="11">
-        <f t="shared" si="3"/>
-        <v>30.397520628000002</v>
+      <c r="E51" s="18">
+        <v>0</v>
       </c>
       <c r="F51" s="2">
         <v>1</v>
@@ -3801,19 +3746,19 @@
         <v>1.9552E-2</v>
       </c>
       <c r="O51">
+        <f t="shared" si="4"/>
+        <v>6.2715999999999994E-2</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="3"/>
+        <v>-2.4447000000000003E-2</v>
+      </c>
+      <c r="Q51">
         <f t="shared" si="5"/>
-        <v>6.2715999999999994E-2</v>
-      </c>
-      <c r="P51">
-        <f t="shared" si="4"/>
-        <v>-2.4447000000000003E-2</v>
-      </c>
-      <c r="Q51">
+        <v>0.17668149999999999</v>
+      </c>
+      <c r="R51">
         <f t="shared" si="6"/>
-        <v>0.17668149999999999</v>
-      </c>
-      <c r="R51">
-        <f t="shared" si="7"/>
         <v>7.2880500000000001E-2</v>
       </c>
     </row>
@@ -3830,9 +3775,8 @@
       <c r="D52" s="3">
         <v>18</v>
       </c>
-      <c r="E52" s="11">
-        <f t="shared" si="3"/>
-        <v>26.267269286999998</v>
+      <c r="E52" s="18">
+        <v>0</v>
       </c>
       <c r="F52" s="2">
         <v>1</v>
@@ -3862,19 +3806,19 @@
         <v>6.6969999999999998E-3</v>
       </c>
       <c r="O52">
+        <f t="shared" si="4"/>
+        <v>-6.5981499999999998E-2</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="3"/>
+        <v>-1.7991500000000001E-2</v>
+      </c>
+      <c r="Q52">
         <f t="shared" si="5"/>
-        <v>-6.5981499999999998E-2</v>
-      </c>
-      <c r="P52">
-        <f t="shared" si="4"/>
-        <v>-1.7991500000000001E-2</v>
-      </c>
-      <c r="Q52">
+        <v>-0.104079</v>
+      </c>
+      <c r="R52">
         <f t="shared" si="6"/>
-        <v>-0.104079</v>
-      </c>
-      <c r="R52">
-        <f t="shared" si="7"/>
         <v>-0.16324549999999999</v>
       </c>
     </row>
@@ -3891,9 +3835,8 @@
       <c r="D53" s="3">
         <v>20</v>
       </c>
-      <c r="E53" s="11">
-        <f t="shared" si="3"/>
-        <v>27.722397643000001</v>
+      <c r="E53" s="18">
+        <v>24</v>
       </c>
       <c r="F53" s="2">
         <v>1</v>
@@ -3923,19 +3866,19 @@
         <v>4.1669999999999997E-3</v>
       </c>
       <c r="O53">
+        <f t="shared" si="4"/>
+        <v>-2.5538999999999999E-2</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="3"/>
+        <v>-1.711E-2</v>
+      </c>
+      <c r="Q53">
         <f t="shared" si="5"/>
-        <v>-2.5538999999999999E-2</v>
-      </c>
-      <c r="P53">
-        <f t="shared" si="4"/>
-        <v>-1.711E-2</v>
-      </c>
-      <c r="Q53">
+        <v>0.21639549999999999</v>
+      </c>
+      <c r="R53">
         <f t="shared" si="6"/>
-        <v>0.21639549999999999</v>
-      </c>
-      <c r="R53">
-        <f t="shared" si="7"/>
         <v>0.136488</v>
       </c>
     </row>
@@ -3952,9 +3895,8 @@
       <c r="D54" s="3">
         <v>21</v>
       </c>
-      <c r="E54" s="11">
-        <f t="shared" si="3"/>
-        <v>33.399481039999998</v>
+      <c r="E54" s="18">
+        <v>0</v>
       </c>
       <c r="F54" s="2">
         <v>1</v>
@@ -3984,19 +3926,19 @@
         <v>8.0058000000000004E-2</v>
       </c>
       <c r="O54">
+        <f t="shared" si="4"/>
+        <v>2.03115E-2</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="3"/>
+        <v>6.5834000000000004E-2</v>
+      </c>
+      <c r="Q54">
         <f t="shared" si="5"/>
-        <v>2.03115E-2</v>
-      </c>
-      <c r="P54">
-        <f t="shared" si="4"/>
-        <v>6.5834000000000004E-2</v>
-      </c>
-      <c r="Q54">
+        <v>0.1026715</v>
+      </c>
+      <c r="R54">
         <f t="shared" si="6"/>
-        <v>0.1026715</v>
-      </c>
-      <c r="R54">
-        <f t="shared" si="7"/>
         <v>2.2243500000000003E-2</v>
       </c>
     </row>
@@ -4013,9 +3955,8 @@
       <c r="D55" s="3">
         <v>20</v>
       </c>
-      <c r="E55" s="11">
-        <f t="shared" si="3"/>
-        <v>28.407680970999998</v>
+      <c r="E55" s="18">
+        <v>50</v>
       </c>
       <c r="F55" s="2">
         <v>1</v>
@@ -4045,19 +3986,19 @@
         <v>-2.7099999999999997E-4</v>
       </c>
       <c r="O55">
+        <f t="shared" si="4"/>
+        <v>2.0958499999999998E-2</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="3"/>
+        <v>2.7310999999999998E-2</v>
+      </c>
+      <c r="Q55">
         <f t="shared" si="5"/>
-        <v>2.0958499999999998E-2</v>
-      </c>
-      <c r="P55">
-        <f t="shared" si="4"/>
-        <v>2.7310999999999998E-2</v>
-      </c>
-      <c r="Q55">
+        <v>-0.1577345</v>
+      </c>
+      <c r="R55">
         <f t="shared" si="6"/>
-        <v>-0.1577345</v>
-      </c>
-      <c r="R55">
-        <f t="shared" si="7"/>
         <v>-0.2337545</v>
       </c>
     </row>
@@ -4074,9 +4015,8 @@
       <c r="D56" s="3">
         <v>19</v>
       </c>
-      <c r="E56" s="11">
-        <f t="shared" si="3"/>
-        <v>27.538233206000001</v>
+      <c r="E56" s="18">
+        <v>32</v>
       </c>
       <c r="F56" s="2">
         <v>1</v>
@@ -4106,19 +4046,19 @@
         <v>6.0911E-2</v>
       </c>
       <c r="O56">
+        <f t="shared" si="4"/>
+        <v>4.812799999999999E-2</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="3"/>
+        <v>6.3338000000000005E-2</v>
+      </c>
+      <c r="Q56">
         <f t="shared" si="5"/>
-        <v>4.812799999999999E-2</v>
-      </c>
-      <c r="P56">
-        <f t="shared" si="4"/>
-        <v>6.3338000000000005E-2</v>
-      </c>
-      <c r="Q56">
+        <v>0.16419149999999999</v>
+      </c>
+      <c r="R56">
         <f t="shared" si="6"/>
-        <v>0.16419149999999999</v>
-      </c>
-      <c r="R56">
-        <f t="shared" si="7"/>
         <v>0.1382755</v>
       </c>
     </row>
@@ -4135,9 +4075,8 @@
       <c r="D57" s="3">
         <v>19</v>
       </c>
-      <c r="E57" s="11">
-        <f t="shared" si="3"/>
-        <v>28.547210065000002</v>
+      <c r="E57" s="18">
+        <v>0</v>
       </c>
       <c r="F57" s="2">
         <v>1</v>
@@ -4167,19 +4106,19 @@
         <v>-7.2345000000000007E-2</v>
       </c>
       <c r="O57">
+        <f t="shared" si="4"/>
+        <v>-3.5323E-2</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="3"/>
+        <v>-7.2483000000000006E-2</v>
+      </c>
+      <c r="Q57">
         <f t="shared" si="5"/>
-        <v>-3.5323E-2</v>
-      </c>
-      <c r="P57">
-        <f t="shared" si="4"/>
-        <v>-7.2483000000000006E-2</v>
-      </c>
-      <c r="Q57">
+        <v>-0.16868549999999999</v>
+      </c>
+      <c r="R57">
         <f t="shared" si="6"/>
-        <v>-0.16868549999999999</v>
-      </c>
-      <c r="R57">
-        <f t="shared" si="7"/>
         <v>-0.13276350000000001</v>
       </c>
     </row>
@@ -4196,9 +4135,8 @@
       <c r="D58" s="3">
         <v>20</v>
       </c>
-      <c r="E58" s="11">
-        <f t="shared" si="3"/>
-        <v>25.649759837000001</v>
+      <c r="E58" s="18">
+        <v>32</v>
       </c>
       <c r="F58" s="2">
         <v>1</v>
@@ -4228,19 +4166,19 @@
         <v>4.8473000000000002E-2</v>
       </c>
       <c r="O58">
+        <f t="shared" si="4"/>
+        <v>4.5471999999999999E-2</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="3"/>
+        <v>6.9178000000000003E-2</v>
+      </c>
+      <c r="Q58">
         <f t="shared" si="5"/>
-        <v>4.5471999999999999E-2</v>
-      </c>
-      <c r="P58">
-        <f t="shared" si="4"/>
-        <v>6.9178000000000003E-2</v>
-      </c>
-      <c r="Q58">
+        <v>0.108737</v>
+      </c>
+      <c r="R58">
         <f t="shared" si="6"/>
-        <v>0.108737</v>
-      </c>
-      <c r="R58">
-        <f t="shared" si="7"/>
         <v>3.3605500000000003E-2</v>
       </c>
     </row>
@@ -4257,9 +4195,8 @@
       <c r="D59" s="3">
         <v>19</v>
       </c>
-      <c r="E59" s="11">
-        <f t="shared" si="3"/>
-        <v>28.222083269999999</v>
+      <c r="E59" s="18">
+        <v>42</v>
       </c>
       <c r="F59" s="2">
         <v>1</v>
@@ -4289,19 +4226,19 @@
         <v>1.6598999999999999E-2</v>
       </c>
       <c r="O59">
+        <f t="shared" si="4"/>
+        <v>2.0188000000000001E-2</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="3"/>
+        <v>-1.33305E-2</v>
+      </c>
+      <c r="Q59">
         <f t="shared" si="5"/>
-        <v>2.0188000000000001E-2</v>
-      </c>
-      <c r="P59">
-        <f t="shared" si="4"/>
-        <v>-1.33305E-2</v>
-      </c>
-      <c r="Q59">
+        <v>4.2142499999999999E-2</v>
+      </c>
+      <c r="R59">
         <f t="shared" si="6"/>
-        <v>4.2142499999999999E-2</v>
-      </c>
-      <c r="R59">
-        <f t="shared" si="7"/>
         <v>-4.95115E-2</v>
       </c>
     </row>
@@ -4318,9 +4255,8 @@
       <c r="D60" s="3">
         <v>22</v>
       </c>
-      <c r="E60" s="11">
-        <f t="shared" si="3"/>
-        <v>31.075425877000001</v>
+      <c r="E60" s="18">
+        <v>4</v>
       </c>
       <c r="F60" s="2">
         <v>1</v>
@@ -4350,19 +4286,19 @@
         <v>4.0099999999999997E-2</v>
       </c>
       <c r="O60">
+        <f t="shared" si="4"/>
+        <v>-2.2508999999999994E-2</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="3"/>
+        <v>1.7735499999999998E-2</v>
+      </c>
+      <c r="Q60">
         <f t="shared" si="5"/>
-        <v>-2.2508999999999994E-2</v>
-      </c>
-      <c r="P60">
-        <f t="shared" si="4"/>
-        <v>1.7735499999999998E-2</v>
-      </c>
-      <c r="Q60">
+        <v>7.3749499999999996E-2</v>
+      </c>
+      <c r="R60">
         <f t="shared" si="6"/>
-        <v>7.3749499999999996E-2</v>
-      </c>
-      <c r="R60">
-        <f t="shared" si="7"/>
         <v>0.123367</v>
       </c>
     </row>
@@ -4379,9 +4315,8 @@
       <c r="D61" s="3">
         <v>18</v>
       </c>
-      <c r="E61" s="11">
-        <f t="shared" si="3"/>
-        <v>30.455561510000003</v>
+      <c r="E61" s="18">
+        <v>25</v>
       </c>
       <c r="F61" s="2">
         <v>1</v>
@@ -4411,19 +4346,19 @@
         <v>0.19259299999999999</v>
       </c>
       <c r="O61">
+        <f t="shared" si="4"/>
+        <v>0.23388150000000002</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="3"/>
+        <v>0.14033000000000001</v>
+      </c>
+      <c r="Q61">
         <f t="shared" si="5"/>
-        <v>0.23388150000000002</v>
-      </c>
-      <c r="P61">
-        <f t="shared" si="4"/>
-        <v>0.14033000000000001</v>
-      </c>
-      <c r="Q61">
+        <v>9.0142E-2</v>
+      </c>
+      <c r="R61">
         <f t="shared" si="6"/>
-        <v>9.0142E-2</v>
-      </c>
-      <c r="R61">
-        <f t="shared" si="7"/>
         <v>0.14987149999999999</v>
       </c>
     </row>
@@ -4440,9 +4375,8 @@
       <c r="D62" s="3">
         <v>32</v>
       </c>
-      <c r="E62" s="11">
-        <f t="shared" si="3"/>
-        <v>41.590708190000001</v>
+      <c r="E62" s="18">
+        <v>0</v>
       </c>
       <c r="F62" s="2">
         <v>1</v>
@@ -4472,19 +4406,19 @@
         <v>-6.5240999999999993E-2</v>
       </c>
       <c r="O62">
+        <f t="shared" si="4"/>
+        <v>-2.8428500000000002E-2</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="3"/>
+        <v>-6.3338999999999993E-2</v>
+      </c>
+      <c r="Q62">
         <f t="shared" si="5"/>
-        <v>-2.8428500000000002E-2</v>
-      </c>
-      <c r="P62">
-        <f t="shared" si="4"/>
-        <v>-6.3338999999999993E-2</v>
-      </c>
-      <c r="Q62">
+        <v>-0.12122250000000001</v>
+      </c>
+      <c r="R62">
         <f t="shared" si="6"/>
-        <v>-0.12122250000000001</v>
-      </c>
-      <c r="R62">
-        <f t="shared" si="7"/>
         <v>-9.6172999999999995E-2</v>
       </c>
     </row>
@@ -4501,9 +4435,8 @@
       <c r="D63" s="3">
         <v>20</v>
       </c>
-      <c r="E63" s="11">
-        <f t="shared" si="3"/>
-        <v>28.071761545000001</v>
+      <c r="E63" s="18">
+        <v>19</v>
       </c>
       <c r="F63" s="2">
         <v>1</v>
@@ -4533,19 +4466,19 @@
         <v>-1.9386E-2</v>
       </c>
       <c r="O63">
+        <f t="shared" si="4"/>
+        <v>-3.1807500000000002E-2</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="3"/>
+        <v>4.6154999999999998E-3</v>
+      </c>
+      <c r="Q63">
         <f t="shared" si="5"/>
-        <v>-3.1807500000000002E-2</v>
-      </c>
-      <c r="P63">
-        <f t="shared" si="4"/>
-        <v>4.6154999999999998E-3</v>
-      </c>
-      <c r="Q63">
+        <v>6.5114499999999992E-2</v>
+      </c>
+      <c r="R63">
         <f t="shared" si="6"/>
-        <v>6.5114499999999992E-2</v>
-      </c>
-      <c r="R63">
-        <f t="shared" si="7"/>
         <v>0.15516199999999999</v>
       </c>
     </row>
@@ -4562,9 +4495,8 @@
       <c r="D64" s="3">
         <v>20</v>
       </c>
-      <c r="E64" s="11">
-        <f t="shared" si="3"/>
-        <v>27.342681935999998</v>
+      <c r="E64" s="18">
+        <v>55</v>
       </c>
       <c r="F64" s="2">
         <v>1</v>
@@ -4594,19 +4526,19 @@
         <v>8.5773000000000002E-2</v>
       </c>
       <c r="O64">
+        <f t="shared" si="4"/>
+        <v>0.1047535</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="3"/>
+        <v>5.3642500000000003E-2</v>
+      </c>
+      <c r="Q64">
         <f t="shared" si="5"/>
-        <v>0.1047535</v>
-      </c>
-      <c r="P64">
-        <f t="shared" si="4"/>
-        <v>5.3642500000000003E-2</v>
-      </c>
-      <c r="Q64">
+        <v>0.14030500000000001</v>
+      </c>
+      <c r="R64">
         <f t="shared" si="6"/>
-        <v>0.14030500000000001</v>
-      </c>
-      <c r="R64">
-        <f t="shared" si="7"/>
         <v>-6.7985000000000004E-2</v>
       </c>
     </row>
@@ -4623,9 +4555,8 @@
       <c r="D65" s="3">
         <v>18</v>
       </c>
-      <c r="E65" s="11">
-        <f t="shared" si="3"/>
-        <v>24.414532676</v>
+      <c r="E65" s="18">
+        <v>3</v>
       </c>
       <c r="F65" s="2">
         <v>1</v>
@@ -4655,19 +4586,19 @@
         <v>6.8507999999999999E-2</v>
       </c>
       <c r="O65">
+        <f t="shared" si="4"/>
+        <v>2.034E-2</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="3"/>
+        <v>4.8063000000000002E-2</v>
+      </c>
+      <c r="Q65">
         <f t="shared" si="5"/>
-        <v>2.034E-2</v>
-      </c>
-      <c r="P65">
-        <f t="shared" si="4"/>
-        <v>4.8063000000000002E-2</v>
-      </c>
-      <c r="Q65">
+        <v>0.10000450000000001</v>
+      </c>
+      <c r="R65">
         <f t="shared" si="6"/>
-        <v>0.10000450000000001</v>
-      </c>
-      <c r="R65">
-        <f t="shared" si="7"/>
         <v>0.12936</v>
       </c>
     </row>
@@ -4684,9 +4615,8 @@
       <c r="D66" s="3">
         <v>35</v>
       </c>
-      <c r="E66" s="11">
-        <f t="shared" si="3"/>
-        <v>42.593527115999997</v>
+      <c r="E66" s="18">
+        <v>0</v>
       </c>
       <c r="F66" s="2">
         <v>1</v>
@@ -4716,19 +4646,19 @@
         <v>4.7199999999999998E-4</v>
       </c>
       <c r="O66">
-        <f t="shared" ref="O66:O71" si="8">AVERAGE(G66,H66)</f>
+        <f t="shared" ref="O66:O71" si="7">AVERAGE(G66,H66)</f>
         <v>-9.7470000000000005E-3</v>
       </c>
       <c r="P66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2.8475000000000002E-3</v>
       </c>
       <c r="Q66">
+        <f t="shared" si="5"/>
+        <v>0.2201245</v>
+      </c>
+      <c r="R66">
         <f t="shared" si="6"/>
-        <v>0.2201245</v>
-      </c>
-      <c r="R66">
-        <f t="shared" si="7"/>
         <v>0.1681745</v>
       </c>
     </row>
@@ -4745,9 +4675,8 @@
       <c r="D67" s="3">
         <v>27</v>
       </c>
-      <c r="E67" s="11">
-        <f t="shared" ref="E67:E71" si="9">SUM(A67,B67,D67)</f>
-        <v>33.086239947000003</v>
+      <c r="E67" s="18">
+        <v>43</v>
       </c>
       <c r="F67" s="2">
         <v>1</v>
@@ -4777,19 +4706,19 @@
         <v>7.8109999999999999E-2</v>
       </c>
       <c r="O67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.12726299999999999</v>
       </c>
       <c r="P67">
-        <f t="shared" ref="P67:P71" si="10">AVERAGE(M67,N67)</f>
+        <f t="shared" ref="P67:P71" si="8">AVERAGE(M67,N67)</f>
         <v>6.7236500000000005E-2</v>
       </c>
       <c r="Q67">
-        <f t="shared" ref="Q67:Q71" si="11">AVERAGE(K67,L67)</f>
+        <f t="shared" ref="Q67:Q71" si="9">AVERAGE(K67,L67)</f>
         <v>1.07595E-2</v>
       </c>
       <c r="R67">
-        <f t="shared" ref="R67:R71" si="12">AVERAGE(I67,J67)</f>
+        <f t="shared" ref="R67:R71" si="10">AVERAGE(I67,J67)</f>
         <v>-1.8960499999999998E-2</v>
       </c>
     </row>
@@ -4806,9 +4735,8 @@
       <c r="D68" s="3">
         <v>21</v>
       </c>
-      <c r="E68" s="11">
-        <f t="shared" si="9"/>
-        <v>28.081494340999999</v>
+      <c r="E68" s="18">
+        <v>42</v>
       </c>
       <c r="F68" s="2">
         <v>1</v>
@@ -4838,19 +4766,19 @@
         <v>3.7670000000000002E-2</v>
       </c>
       <c r="O68">
+        <f t="shared" si="7"/>
+        <v>0.25682749999999999</v>
+      </c>
+      <c r="P68">
         <f t="shared" si="8"/>
-        <v>0.25682749999999999</v>
-      </c>
-      <c r="P68">
+        <v>-1.8767499999999996E-2</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="9"/>
+        <v>-5.6598999999999997E-2</v>
+      </c>
+      <c r="R68">
         <f t="shared" si="10"/>
-        <v>-1.8767499999999996E-2</v>
-      </c>
-      <c r="Q68">
-        <f t="shared" si="11"/>
-        <v>-5.6598999999999997E-2</v>
-      </c>
-      <c r="R68">
-        <f t="shared" si="12"/>
         <v>0.17669699999999999</v>
       </c>
     </row>
@@ -4867,9 +4795,8 @@
       <c r="D69" s="3">
         <v>22</v>
       </c>
-      <c r="E69" s="11">
-        <f t="shared" si="9"/>
-        <v>32.586067829999998</v>
+      <c r="E69" s="18">
+        <v>35</v>
       </c>
       <c r="F69" s="2">
         <v>1</v>
@@ -4899,19 +4826,19 @@
         <v>6.2628000000000003E-2</v>
       </c>
       <c r="O69">
+        <f t="shared" si="7"/>
+        <v>-6.6050499999999998E-2</v>
+      </c>
+      <c r="P69">
         <f t="shared" si="8"/>
-        <v>-6.6050499999999998E-2</v>
-      </c>
-      <c r="P69">
+        <v>1.1983000000000001E-2</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="9"/>
+        <v>-7.7405499999999988E-2</v>
+      </c>
+      <c r="R69">
         <f t="shared" si="10"/>
-        <v>1.1983000000000001E-2</v>
-      </c>
-      <c r="Q69">
-        <f t="shared" si="11"/>
-        <v>-7.7405499999999988E-2</v>
-      </c>
-      <c r="R69">
-        <f t="shared" si="12"/>
         <v>-7.613049999999999E-2</v>
       </c>
     </row>
@@ -4928,9 +4855,8 @@
       <c r="D70" s="3">
         <v>23</v>
       </c>
-      <c r="E70" s="11">
-        <f t="shared" si="9"/>
-        <v>34.051443660000004</v>
+      <c r="E70" s="18">
+        <v>9</v>
       </c>
       <c r="F70" s="2">
         <v>1</v>
@@ -4960,19 +4886,19 @@
         <v>-5.527E-2</v>
       </c>
       <c r="O70">
+        <f t="shared" si="7"/>
+        <v>-0.23227700000000001</v>
+      </c>
+      <c r="P70">
         <f t="shared" si="8"/>
-        <v>-0.23227700000000001</v>
-      </c>
-      <c r="P70">
+        <v>-0.110206</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="9"/>
+        <v>-4.8635500000000005E-2</v>
+      </c>
+      <c r="R70">
         <f t="shared" si="10"/>
-        <v>-0.110206</v>
-      </c>
-      <c r="Q70">
-        <f t="shared" si="11"/>
-        <v>-4.8635500000000005E-2</v>
-      </c>
-      <c r="R70">
-        <f t="shared" si="12"/>
         <v>-2.8743999999999999E-2</v>
       </c>
     </row>
@@ -4980,7 +4906,7 @@
       <c r="A71" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B71" s="14">
+      <c r="B71" s="12">
         <v>6.4567896820000001</v>
       </c>
       <c r="C71" s="4">
@@ -4989,9 +4915,8 @@
       <c r="D71" s="7">
         <v>19</v>
       </c>
-      <c r="E71" s="12">
-        <f t="shared" si="9"/>
-        <v>25.456789682</v>
+      <c r="E71" s="18">
+        <v>26</v>
       </c>
       <c r="F71" s="5">
         <v>1</v>
@@ -5021,19 +4946,19 @@
         <v>0.190882</v>
       </c>
       <c r="O71" s="6">
+        <f t="shared" si="7"/>
+        <v>0.16444400000000001</v>
+      </c>
+      <c r="P71" s="6">
         <f t="shared" si="8"/>
-        <v>0.16444400000000001</v>
-      </c>
-      <c r="P71" s="6">
+        <v>0.161913</v>
+      </c>
+      <c r="Q71" s="6">
+        <f t="shared" si="9"/>
+        <v>-8.0625000000000002E-3</v>
+      </c>
+      <c r="R71" s="6">
         <f t="shared" si="10"/>
-        <v>0.161913</v>
-      </c>
-      <c r="Q71" s="6">
-        <f t="shared" si="11"/>
-        <v>-8.0625000000000002E-3</v>
-      </c>
-      <c r="R71" s="6">
-        <f t="shared" si="12"/>
         <v>1.48185E-2</v>
       </c>
     </row>

</xml_diff>